<commit_message>
reverting matlabtesting multiple solver
</commit_message>
<xml_diff>
--- a/Dokumente/project plan.xlsx
+++ b/Dokumente/project plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A0048C-DB1D-4F6D-A38F-A7AC3FCC8624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5F0AAE-2FB0-447E-9C73-262AC1D7CC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1199,6 +1199,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="17" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="18" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="174" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="173" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1218,30 +1242,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="174" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="43" borderId="20" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="43" borderId="17" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="43" borderId="18" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="39" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="39" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
@@ -1815,7 +1815,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1869,146 +1869,146 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="H3" s="62">
+      <c r="H3" s="70">
         <f>H4</f>
         <v>45922</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="62">
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="70">
         <f>O4</f>
         <v>45929</v>
       </c>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="62">
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="70">
         <f t="shared" ref="V3" si="0">V4</f>
         <v>45936</v>
       </c>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="62">
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="72"/>
+      <c r="AC3" s="70">
         <f t="shared" ref="AC3" si="1">AC4</f>
         <v>45943</v>
       </c>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
-      <c r="AH3" s="63"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="62">
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="72"/>
+      <c r="AJ3" s="70">
         <f t="shared" ref="AJ3" si="2">AJ4</f>
         <v>45950</v>
       </c>
-      <c r="AK3" s="63"/>
-      <c r="AL3" s="63"/>
-      <c r="AM3" s="63"/>
-      <c r="AN3" s="63"/>
-      <c r="AO3" s="63"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="62">
+      <c r="AK3" s="71"/>
+      <c r="AL3" s="71"/>
+      <c r="AM3" s="71"/>
+      <c r="AN3" s="71"/>
+      <c r="AO3" s="71"/>
+      <c r="AP3" s="72"/>
+      <c r="AQ3" s="70">
         <f t="shared" ref="AQ3" si="3">AQ4</f>
         <v>45957</v>
       </c>
-      <c r="AR3" s="63"/>
-      <c r="AS3" s="63"/>
-      <c r="AT3" s="63"/>
-      <c r="AU3" s="63"/>
-      <c r="AV3" s="63"/>
-      <c r="AW3" s="64"/>
-      <c r="AX3" s="62">
+      <c r="AR3" s="71"/>
+      <c r="AS3" s="71"/>
+      <c r="AT3" s="71"/>
+      <c r="AU3" s="71"/>
+      <c r="AV3" s="71"/>
+      <c r="AW3" s="72"/>
+      <c r="AX3" s="70">
         <f t="shared" ref="AX3" si="4">AX4</f>
         <v>45964</v>
       </c>
-      <c r="AY3" s="63"/>
-      <c r="AZ3" s="63"/>
-      <c r="BA3" s="63"/>
-      <c r="BB3" s="63"/>
-      <c r="BC3" s="63"/>
-      <c r="BD3" s="64"/>
-      <c r="BE3" s="62">
+      <c r="AY3" s="71"/>
+      <c r="AZ3" s="71"/>
+      <c r="BA3" s="71"/>
+      <c r="BB3" s="71"/>
+      <c r="BC3" s="71"/>
+      <c r="BD3" s="72"/>
+      <c r="BE3" s="70">
         <f t="shared" ref="BE3" si="5">BE4</f>
         <v>45971</v>
       </c>
-      <c r="BF3" s="63"/>
-      <c r="BG3" s="63"/>
-      <c r="BH3" s="63"/>
-      <c r="BI3" s="63"/>
-      <c r="BJ3" s="63"/>
-      <c r="BK3" s="64"/>
-      <c r="BL3" s="62">
+      <c r="BF3" s="71"/>
+      <c r="BG3" s="71"/>
+      <c r="BH3" s="71"/>
+      <c r="BI3" s="71"/>
+      <c r="BJ3" s="71"/>
+      <c r="BK3" s="72"/>
+      <c r="BL3" s="70">
         <f t="shared" ref="BL3" si="6">BL4</f>
         <v>45978</v>
       </c>
-      <c r="BM3" s="63"/>
-      <c r="BN3" s="63"/>
-      <c r="BO3" s="63"/>
-      <c r="BP3" s="63"/>
-      <c r="BQ3" s="63"/>
-      <c r="BR3" s="64"/>
-      <c r="BS3" s="62">
+      <c r="BM3" s="71"/>
+      <c r="BN3" s="71"/>
+      <c r="BO3" s="71"/>
+      <c r="BP3" s="71"/>
+      <c r="BQ3" s="71"/>
+      <c r="BR3" s="72"/>
+      <c r="BS3" s="70">
         <f t="shared" ref="BS3" si="7">BS4</f>
         <v>45985</v>
       </c>
-      <c r="BT3" s="63"/>
-      <c r="BU3" s="63"/>
-      <c r="BV3" s="63"/>
-      <c r="BW3" s="63"/>
-      <c r="BX3" s="63"/>
-      <c r="BY3" s="64"/>
-      <c r="BZ3" s="62">
+      <c r="BT3" s="71"/>
+      <c r="BU3" s="71"/>
+      <c r="BV3" s="71"/>
+      <c r="BW3" s="71"/>
+      <c r="BX3" s="71"/>
+      <c r="BY3" s="72"/>
+      <c r="BZ3" s="70">
         <f t="shared" ref="BZ3" si="8">BZ4</f>
         <v>45992</v>
       </c>
-      <c r="CA3" s="63"/>
-      <c r="CB3" s="63"/>
-      <c r="CC3" s="63"/>
-      <c r="CD3" s="63"/>
-      <c r="CE3" s="63"/>
-      <c r="CF3" s="64"/>
-      <c r="CG3" s="62">
+      <c r="CA3" s="71"/>
+      <c r="CB3" s="71"/>
+      <c r="CC3" s="71"/>
+      <c r="CD3" s="71"/>
+      <c r="CE3" s="71"/>
+      <c r="CF3" s="72"/>
+      <c r="CG3" s="70">
         <f t="shared" ref="CG3" si="9">CG4</f>
         <v>45999</v>
       </c>
-      <c r="CH3" s="63"/>
-      <c r="CI3" s="63"/>
-      <c r="CJ3" s="63"/>
-      <c r="CK3" s="63"/>
-      <c r="CL3" s="63"/>
-      <c r="CM3" s="64"/>
-      <c r="CN3" s="62">
+      <c r="CH3" s="71"/>
+      <c r="CI3" s="71"/>
+      <c r="CJ3" s="71"/>
+      <c r="CK3" s="71"/>
+      <c r="CL3" s="71"/>
+      <c r="CM3" s="72"/>
+      <c r="CN3" s="70">
         <f t="shared" ref="CN3" si="10">CN4</f>
         <v>46006</v>
       </c>
-      <c r="CO3" s="63"/>
-      <c r="CP3" s="63"/>
-      <c r="CQ3" s="63"/>
-      <c r="CR3" s="63"/>
-      <c r="CS3" s="63"/>
-      <c r="CT3" s="64"/>
-      <c r="CU3" s="62">
+      <c r="CO3" s="71"/>
+      <c r="CP3" s="71"/>
+      <c r="CQ3" s="71"/>
+      <c r="CR3" s="71"/>
+      <c r="CS3" s="71"/>
+      <c r="CT3" s="72"/>
+      <c r="CU3" s="70">
         <f t="shared" ref="CU3" si="11">CU4</f>
         <v>46013</v>
       </c>
-      <c r="CV3" s="63"/>
-      <c r="CW3" s="63"/>
-      <c r="CX3" s="63"/>
-      <c r="CY3" s="63"/>
-      <c r="CZ3" s="63"/>
-      <c r="DA3" s="64"/>
+      <c r="CV3" s="71"/>
+      <c r="CW3" s="71"/>
+      <c r="CX3" s="71"/>
+      <c r="CY3" s="71"/>
+      <c r="CZ3" s="71"/>
+      <c r="DA3" s="72"/>
     </row>
     <row r="4" spans="1:105" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3054,7 +3054,7 @@
     </row>
     <row r="8" spans="1:105" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="75" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="35" t="s">
@@ -3172,7 +3172,7 @@
     </row>
     <row r="9" spans="1:105" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
-      <c r="B9" s="68"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="35" t="s">
         <v>36</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="75" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="35" t="s">
@@ -3408,7 +3408,7 @@
     </row>
     <row r="11" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="68"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="35" t="s">
         <v>36</v>
       </c>
@@ -3526,7 +3526,7 @@
       <c r="A12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="75" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="35" t="s">
@@ -3644,7 +3644,7 @@
     </row>
     <row r="13" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
-      <c r="B13" s="68"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="35" t="s">
         <v>36</v>
       </c>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="15" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="73" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="58" t="s">
@@ -3989,7 +3989,7 @@
     </row>
     <row r="16" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="66"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="58" t="s">
         <v>36</v>
       </c>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="17" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="73" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="58" t="s">
@@ -4220,7 +4220,7 @@
     </row>
     <row r="18" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
-      <c r="B18" s="66"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="58" t="s">
         <v>36</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>45936</v>
       </c>
       <c r="E18" s="39">
-        <v>45949</v>
+        <v>45952</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="19" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="73" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="58" t="s">
@@ -4451,7 +4451,7 @@
     </row>
     <row r="20" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
-      <c r="B20" s="66"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="58" t="s">
         <v>36</v>
       </c>
@@ -4459,12 +4459,12 @@
         <v>45936</v>
       </c>
       <c r="E20" s="39">
-        <v>45949</v>
+        <v>45952</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10">
         <f t="shared" si="48"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="22" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="62" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="43" t="s">
@@ -4796,16 +4796,20 @@
     </row>
     <row r="23" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
-      <c r="B23" s="76"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
+      <c r="D23" s="44">
+        <v>45951</v>
+      </c>
+      <c r="E23" s="44">
+        <v>45957</v>
+      </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="10" t="str">
+      <c r="G23" s="10">
         <f t="shared" si="48"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
@@ -4908,7 +4912,7 @@
     </row>
     <row r="24" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="62" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="43" t="s">
@@ -5026,16 +5030,20 @@
     </row>
     <row r="25" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
-      <c r="B25" s="76"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
+      <c r="D25" s="44">
+        <v>45953</v>
+      </c>
+      <c r="E25" s="44">
+        <v>45957</v>
+      </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="10" t="str">
+      <c r="G25" s="10">
         <f t="shared" si="48"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
@@ -5138,7 +5146,7 @@
     </row>
     <row r="26" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="62" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="43" t="s">
@@ -5256,16 +5264,20 @@
     </row>
     <row r="27" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
-      <c r="B27" s="76"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
+      <c r="D27" s="44">
+        <v>45953</v>
+      </c>
+      <c r="E27" s="44">
+        <v>45957</v>
+      </c>
       <c r="F27" s="10"/>
-      <c r="G27" s="10" t="str">
+      <c r="G27" s="10">
         <f t="shared" si="48"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
@@ -5477,7 +5489,7 @@
     </row>
     <row r="29" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="67" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="48" t="s">
@@ -5595,7 +5607,7 @@
     </row>
     <row r="30" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
-      <c r="B30" s="74"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="48" t="s">
         <v>36</v>
       </c>
@@ -5707,7 +5719,7 @@
     </row>
     <row r="31" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="67" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="48" t="s">
@@ -5825,7 +5837,7 @@
     </row>
     <row r="32" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
-      <c r="B32" s="74"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="48" t="s">
         <v>36</v>
       </c>
@@ -6048,7 +6060,7 @@
     </row>
     <row r="34" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="64" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="51" t="s">
@@ -6166,7 +6178,7 @@
     </row>
     <row r="35" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
-      <c r="B35" s="72"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="51" t="s">
         <v>36</v>
       </c>
@@ -6278,7 +6290,7 @@
     </row>
     <row r="36" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="64" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="51" t="s">
@@ -6396,7 +6408,7 @@
     </row>
     <row r="37" spans="1:105" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
-      <c r="B37" s="71"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="51" t="s">
         <v>36</v>
       </c>
@@ -6740,24 +6752,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="O3:U3"/>
-    <mergeCell ref="V3:AB3"/>
-    <mergeCell ref="AC3:AI3"/>
-    <mergeCell ref="CU3:DA3"/>
-    <mergeCell ref="BL3:BR3"/>
-    <mergeCell ref="BS3:BY3"/>
-    <mergeCell ref="BZ3:CF3"/>
-    <mergeCell ref="CG3:CM3"/>
-    <mergeCell ref="CN3:CT3"/>
     <mergeCell ref="AQ3:AW3"/>
     <mergeCell ref="AX3:BD3"/>
     <mergeCell ref="BE3:BK3"/>
@@ -6768,6 +6762,24 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B17:B18"/>
+    <mergeCell ref="CU3:DA3"/>
+    <mergeCell ref="BL3:BR3"/>
+    <mergeCell ref="BS3:BY3"/>
+    <mergeCell ref="BZ3:CF3"/>
+    <mergeCell ref="CG3:CM3"/>
+    <mergeCell ref="CN3:CT3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="O3:U3"/>
+    <mergeCell ref="V3:AB3"/>
+    <mergeCell ref="AC3:AI3"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B26:B27"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:DA39">
     <cfRule type="expression" dxfId="3" priority="17">
@@ -6811,6 +6823,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E708E235B0E5CE4EBF02E35118BE8A61" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c9cf5307cf036da9aa5d5eb7826aa596">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="21da7c7b-2a86-4dff-bdbf-913f324e8051" xmlns:ns3="3d8d41c4-2d1a-4f79-aab5-2440921370ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc1ee7d851c350a78eceaa91df4bcabc" ns2:_="" ns3:_="">
     <xsd:import namespace="21da7c7b-2a86-4dff-bdbf-913f324e8051"/>
@@ -7011,15 +7032,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
@@ -7032,6 +7044,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34BE0F69-5617-44E2-9F76-316AC1DD72E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7048,12 +7068,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>